<commit_message>
Update File mẫu import
Update File mẫu import
</commit_message>
<xml_diff>
--- a/src/views/FileMau/FileImportVanBang.xlsx
+++ b/src/views/FileMau/FileImportVanBang.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QLVB_22102023_FE\fe-_qlvb\src\views\FileMau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>STT</t>
   </si>
@@ -294,6 +294,18 @@
   </si>
   <si>
     <t>054201024002</t>
+  </si>
+  <si>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>7,9</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>6,6</t>
   </si>
 </sst>
 </file>
@@ -793,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1090,7 @@
         <v>67</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>82</v>
@@ -1097,7 +1109,7 @@
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="W3" s="13" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>84</v>
@@ -1156,7 +1168,7 @@
         <v>67</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>82</v>
@@ -1180,8 +1192,8 @@
       <c r="X4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Y4" s="13">
-        <v>6</v>
+      <c r="Y4" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>

</xml_diff>

<commit_message>
Thay đổi file mẫu
Thay đổi file mẫu
</commit_message>
<xml_diff>
--- a/src/views/FileMau/FileImportVanBang.xlsx
+++ b/src/views/FileMau/FileImportVanBang.xlsx
@@ -302,10 +302,10 @@
     <t>7,9</t>
   </si>
   <si>
-    <t>8,9</t>
-  </si>
-  <si>
-    <t>6,6</t>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>6.6</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Chỉnh sửa file mẫu
Chỉnh sửa file mẫu
</commit_message>
<xml_diff>
--- a/src/views/FileMau/FileImportVanBang.xlsx
+++ b/src/views/FileMau/FileImportVanBang.xlsx
@@ -296,16 +296,16 @@
     <t>054201024002</t>
   </si>
   <si>
-    <t>7,8</t>
-  </si>
-  <si>
-    <t>7,9</t>
-  </si>
-  <si>
     <t>8.9</t>
   </si>
   <si>
     <t>6.6</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>7.9</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
         <v>67</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>82</v>
@@ -1109,7 +1109,7 @@
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="W3" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>84</v>
@@ -1168,7 +1168,7 @@
         <v>67</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>82</v>
@@ -1193,7 +1193,7 @@
         <v>85</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>

</xml_diff>